<commit_message>
Same Document only Changed Values
</commit_message>
<xml_diff>
--- a/Onur/Analytical_Calculation_Generator.xlsx
+++ b/Onur/Analytical_Calculation_Generator.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oztas/Desktop/projects/EE464-Term-Project-/Onur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF28D2F2-F51D-684C-B766-AC8FEEC09CE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBE0945-4619-0445-A9D7-21FE5AF64FCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16260" xr2:uid="{7971E4F1-08DB-C84F-8FA7-CDE6FD8E1E11}"/>
+    <workbookView xWindow="12000" yWindow="500" windowWidth="16440" windowHeight="16260" xr2:uid="{7971E4F1-08DB-C84F-8FA7-CDE6FD8E1E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -365,44 +365,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,7 +720,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,12 +730,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -744,14 +744,14 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="H3" s="13" t="s">
+      <c r="C3" s="26"/>
+      <c r="H3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -765,7 +765,7 @@
       </c>
       <c r="I4" s="2">
         <f>ROUND((((220+400)/2/12*2*C6)),0)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -780,7 +780,7 @@
       </c>
       <c r="I5" s="2">
         <f>12/C5/2*I4</f>
-        <v>0.35454545454545455</v>
+        <v>0.43636363636363634</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -788,14 +788,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="3">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="2">
         <f>12/C4/2*I4</f>
-        <v>0.19500000000000001</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -806,36 +806,36 @@
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="2">
         <f>(1-2*I5)/32/0.04</f>
-        <v>0.22727272727272727</v>
+        <v>9.9431818181818218E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
       <c r="H8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="2">
         <f>SQRT(I7/C7/C8)</f>
-        <v>10143.219034527579</v>
+        <v>6709.1087647541644</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -845,17 +845,17 @@
       <c r="C9" s="5">
         <v>100000</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
       <c r="H9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="2">
         <f>I7/C9/C9</f>
-        <v>2.2727272727272728E-11</v>
+        <v>9.9431818181818207E-12</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -863,18 +863,18 @@
         <v>10</v>
       </c>
       <c r="C10" s="6">
-        <f>47*10^-6</f>
-        <v>4.6999999999999997E-5</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+        <f>160*10^-6</f>
+        <v>1.5999999999999999E-4</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
       <c r="H10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="2">
         <f>I9/C10</f>
-        <v>4.8355899419729211E-7</v>
+        <v>6.2144886363636381E-8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>